<commit_message>
basic structure and content
</commit_message>
<xml_diff>
--- a/stimuli_data.xlsx
+++ b/stimuli_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="1580" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>stim_nr</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,11 +459,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -485,11 +485,11 @@
       <c r="G3">
         <v>-1</v>
       </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -511,11 +511,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>4</v>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -537,11 +537,11 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -563,11 +563,11 @@
       <c r="G6">
         <v>-1</v>
       </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -589,11 +589,11 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -615,11 +615,11 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -641,11 +641,11 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -667,11 +667,11 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>7</v>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -693,11 +693,11 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>6</v>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -719,11 +719,11 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>4</v>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -745,11 +745,11 @@
       <c r="G13">
         <v>-1</v>
       </c>
-      <c r="H13" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" t="s">
-        <v>5</v>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -771,11 +771,11 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>7</v>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -797,11 +797,11 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" t="s">
-        <v>6</v>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -823,11 +823,11 @@
       <c r="G16">
         <v>-1</v>
       </c>
-      <c r="H16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>4</v>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -849,11 +849,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" t="s">
-        <v>5</v>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>